<commit_message>
favorability_check() only needs 'df' and 'tb' as input
Former-commit-id: 27cae9f3d6b0a0d382dc99c8ebd27cfc7f3c33d4
Former-commit-id: 7772146686362c82ea3f5e17610158c22d61dbf2
</commit_message>
<xml_diff>
--- a/tests/test_tax_transfers/test_data/test_dfs_favorability_check.xlsx
+++ b/tests/test_tax_transfers/test_data/test_dfs_favorability_check.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="W:\izamod\izadynmod\tests\test_tax_transfers\test_data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="W:\izamod\dyn\izadynmod\tests\test_tax_transfers\test_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
   <si>
     <t>hid</t>
   </si>
@@ -80,13 +80,7 @@
     <t>nettax_nokfb_tu</t>
   </si>
   <si>
-    <t>nettax_abg_nokfb_tu</t>
-  </si>
-  <si>
     <t>nettax_kfb_tu</t>
-  </si>
-  <si>
-    <t>nettax_abg_kfb_tu</t>
   </si>
 </sst>
 </file>
@@ -483,10 +477,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:W9"/>
+  <dimension ref="A1:U12"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="O5" sqref="O5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -495,7 +489,7 @@
     <col min="11" max="12" width="14.140625"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -553,14 +547,8 @@
       <c r="U1" t="s">
         <v>18</v>
       </c>
-      <c r="V1" t="s">
-        <v>19</v>
-      </c>
-      <c r="W1" t="s">
-        <v>20</v>
-      </c>
     </row>
-    <row r="2" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
@@ -604,7 +592,7 @@
         <v>2016</v>
       </c>
       <c r="O2" s="3">
-        <f>MIN(T2:W2)/12</f>
+        <f>MIN(T2:U2)/12</f>
         <v>583.33333333333337</v>
       </c>
       <c r="P2" s="1">
@@ -623,19 +611,11 @@
         <v>7672</v>
       </c>
       <c r="U2">
-        <f>G2-12*L2</f>
-        <v>7672</v>
-      </c>
-      <c r="V2">
-        <f t="shared" ref="V2:V9" si="0">H2+J2</f>
+        <f>H2</f>
         <v>7000</v>
       </c>
-      <c r="W2">
-        <f t="shared" ref="W2:W9" si="1">I2</f>
-        <v>7000</v>
-      </c>
     </row>
-    <row r="3" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>1</v>
       </c>
@@ -643,7 +623,7 @@
         <v>1</v>
       </c>
       <c r="C3">
-        <f t="shared" ref="C3:C8" si="2">C2+1</f>
+        <f t="shared" ref="C3:C8" si="0">C2+1</f>
         <v>2</v>
       </c>
       <c r="D3" t="b">
@@ -679,7 +659,7 @@
         <v>2016</v>
       </c>
       <c r="O3" s="3">
-        <f>MIN(T3:W3)/12</f>
+        <f>MIN(T3:U3)/12</f>
         <v>583.33333333333337</v>
       </c>
       <c r="P3" s="1">
@@ -698,27 +678,19 @@
         <v>7672</v>
       </c>
       <c r="U3">
-        <f>G3-12*L3</f>
-        <v>7672</v>
-      </c>
-      <c r="V3">
+        <f t="shared" ref="U3:U9" si="1">H3</f>
+        <v>7000</v>
+      </c>
+    </row>
+    <row r="4" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>1</v>
+      </c>
+      <c r="B4">
+        <v>1</v>
+      </c>
+      <c r="C4">
         <f t="shared" si="0"/>
-        <v>7000</v>
-      </c>
-      <c r="W3">
-        <f t="shared" si="1"/>
-        <v>7000</v>
-      </c>
-    </row>
-    <row r="4" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="A4">
-        <v>1</v>
-      </c>
-      <c r="B4">
-        <v>1</v>
-      </c>
-      <c r="C4">
-        <f t="shared" si="2"/>
         <v>3</v>
       </c>
       <c r="D4" t="b">
@@ -754,7 +726,7 @@
         <v>2016</v>
       </c>
       <c r="O4" s="3">
-        <f>MIN(T4:W4)/12</f>
+        <f>MIN(T4:U4)/12</f>
         <v>0</v>
       </c>
       <c r="P4" s="1">
@@ -772,18 +744,11 @@
         <v>0</v>
       </c>
       <c r="U4">
-        <v>0</v>
-      </c>
-      <c r="V4">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="W4">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>2</v>
       </c>
@@ -791,7 +756,7 @@
         <v>2</v>
       </c>
       <c r="C5">
-        <f t="shared" si="2"/>
+        <f t="shared" si="0"/>
         <v>4</v>
       </c>
       <c r="D5" t="b">
@@ -827,8 +792,8 @@
         <v>2012</v>
       </c>
       <c r="O5" s="3">
-        <f>MIN(T5:W5)/12</f>
-        <v>500</v>
+        <f>F5/12</f>
+        <v>416.66666666666669</v>
       </c>
       <c r="P5" s="1">
         <v>0</v>
@@ -842,23 +807,15 @@
         <v>0</v>
       </c>
       <c r="T5">
-        <f>F5-12*L5+J5</f>
-        <v>8000</v>
+        <f>F5-12*L5+8000</f>
+        <v>13000</v>
       </c>
       <c r="U5">
-        <f>G5-12*L5</f>
-        <v>6000</v>
-      </c>
-      <c r="V5">
-        <f t="shared" si="0"/>
-        <v>8000</v>
-      </c>
-      <c r="W5">
-        <f t="shared" si="1"/>
-        <v>6000</v>
+        <f>H5+8000</f>
+        <v>13000</v>
       </c>
     </row>
-    <row r="6" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>4</v>
       </c>
@@ -866,7 +823,7 @@
         <v>4</v>
       </c>
       <c r="C6">
-        <f t="shared" si="2"/>
+        <f t="shared" si="0"/>
         <v>5</v>
       </c>
       <c r="D6" t="b">
@@ -920,19 +877,11 @@
         <v>15344</v>
       </c>
       <c r="U6">
-        <f>G6-12*L6</f>
-        <v>15344</v>
-      </c>
-      <c r="V6">
-        <f t="shared" si="0"/>
-        <v>18000</v>
-      </c>
-      <c r="W6">
         <f t="shared" si="1"/>
         <v>18000</v>
       </c>
     </row>
-    <row r="7" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>4</v>
       </c>
@@ -940,7 +889,7 @@
         <v>4</v>
       </c>
       <c r="C7">
-        <f t="shared" si="2"/>
+        <f t="shared" si="0"/>
         <v>6</v>
       </c>
       <c r="D7" t="b">
@@ -994,19 +943,11 @@
         <v>15344</v>
       </c>
       <c r="U7">
-        <f>G7-12*L7</f>
-        <v>15344</v>
-      </c>
-      <c r="V7">
-        <f t="shared" si="0"/>
-        <v>18000</v>
-      </c>
-      <c r="W7">
         <f t="shared" si="1"/>
         <v>18000</v>
       </c>
     </row>
-    <row r="8" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>4</v>
       </c>
@@ -1014,7 +955,7 @@
         <v>4</v>
       </c>
       <c r="C8">
-        <f t="shared" si="2"/>
+        <f t="shared" si="0"/>
         <v>7</v>
       </c>
       <c r="D8" t="b">
@@ -1066,18 +1007,11 @@
         <v>0</v>
       </c>
       <c r="U8">
-        <v>0</v>
-      </c>
-      <c r="V8">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="W8">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>4</v>
       </c>
@@ -1136,14 +1070,191 @@
         <v>0</v>
       </c>
       <c r="U9">
-        <v>0</v>
-      </c>
-      <c r="V9">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="W9">
         <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A10">
+        <v>5</v>
+      </c>
+      <c r="B10">
+        <v>5</v>
+      </c>
+      <c r="C10">
+        <v>9</v>
+      </c>
+      <c r="D10" t="b">
+        <v>1</v>
+      </c>
+      <c r="E10" t="b">
+        <v>0</v>
+      </c>
+      <c r="F10">
+        <v>12000</v>
+      </c>
+      <c r="G10">
+        <v>12000</v>
+      </c>
+      <c r="H10">
+        <v>10000</v>
+      </c>
+      <c r="I10">
+        <v>10000</v>
+      </c>
+      <c r="J10">
+        <v>0</v>
+      </c>
+      <c r="K10">
+        <v>0</v>
+      </c>
+      <c r="L10">
+        <v>194</v>
+      </c>
+      <c r="M10">
+        <v>2019</v>
+      </c>
+      <c r="O10" s="3">
+        <f>2*T10/12</f>
+        <v>1612</v>
+      </c>
+      <c r="P10" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q10" s="1">
+        <v>0</v>
+      </c>
+      <c r="R10" s="1">
+        <v>0</v>
+      </c>
+      <c r="T10">
+        <f>F10-(12*L10)</f>
+        <v>9672</v>
+      </c>
+      <c r="U10">
+        <f t="shared" ref="U10" si="2">H10</f>
+        <v>10000</v>
+      </c>
+    </row>
+    <row r="11" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A11">
+        <v>5</v>
+      </c>
+      <c r="B11">
+        <v>5</v>
+      </c>
+      <c r="C11">
+        <v>10</v>
+      </c>
+      <c r="D11" t="b">
+        <v>1</v>
+      </c>
+      <c r="E11" t="b">
+        <v>0</v>
+      </c>
+      <c r="F11">
+        <v>12000</v>
+      </c>
+      <c r="G11">
+        <v>12000</v>
+      </c>
+      <c r="H11">
+        <v>10000</v>
+      </c>
+      <c r="I11">
+        <v>10000</v>
+      </c>
+      <c r="J11">
+        <v>0</v>
+      </c>
+      <c r="K11">
+        <v>0</v>
+      </c>
+      <c r="L11">
+        <v>194</v>
+      </c>
+      <c r="M11">
+        <v>2019</v>
+      </c>
+      <c r="O11" s="3">
+        <f>2*T11/12</f>
+        <v>1612</v>
+      </c>
+      <c r="P11" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q11" s="1">
+        <v>0</v>
+      </c>
+      <c r="R11" s="1">
+        <v>0</v>
+      </c>
+      <c r="T11">
+        <f t="shared" ref="T11:T12" si="3">F11-(12*L11)</f>
+        <v>9672</v>
+      </c>
+      <c r="U11">
+        <f t="shared" ref="U11:U12" si="4">H11</f>
+        <v>10000</v>
+      </c>
+    </row>
+    <row r="12" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A12">
+        <v>5</v>
+      </c>
+      <c r="B12">
+        <v>5</v>
+      </c>
+      <c r="C12">
+        <v>11</v>
+      </c>
+      <c r="D12" t="b">
+        <v>0</v>
+      </c>
+      <c r="E12" t="b">
+        <v>1</v>
+      </c>
+      <c r="F12">
+        <v>0</v>
+      </c>
+      <c r="G12">
+        <v>0</v>
+      </c>
+      <c r="H12">
+        <v>0</v>
+      </c>
+      <c r="I12">
+        <v>0</v>
+      </c>
+      <c r="J12">
+        <v>0</v>
+      </c>
+      <c r="K12">
+        <v>194</v>
+      </c>
+      <c r="L12">
+        <v>194</v>
+      </c>
+      <c r="M12">
+        <v>2019</v>
+      </c>
+      <c r="O12" s="3">
+        <v>0</v>
+      </c>
+      <c r="P12" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q12" s="1">
+        <v>0</v>
+      </c>
+      <c r="R12" s="1">
+        <v>0</v>
+      </c>
+      <c r="T12">
+        <v>0</v>
+      </c>
+      <c r="U12">
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
     </row>

</xml_diff>